<commit_message>
Fixed tilemaps added comments
</commit_message>
<xml_diff>
--- a/Werkbestanden/West Noord.xlsx
+++ b/Werkbestanden/West Noord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\schooljaar2\C2Eindopdracht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsk\OneDrive\Documenten\Stenden\Jaar 2\Periode 4\C2Eindopdracht\Werkbestanden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE465B-55A2-4C51-A812-980451D1F2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC69CBFB-4C0B-4C86-A04C-5084D9B90B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13125" yWindow="1290" windowWidth="19920" windowHeight="12195" xr2:uid="{9793C51D-34E6-41BE-A7FF-8B46D546125D}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="30270" windowHeight="14460" xr2:uid="{9793C51D-34E6-41BE-A7FF-8B46D546125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -462,7 +462,7 @@
   <dimension ref="A1:AH34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -934,10 +934,10 @@
       <c r="M9">
         <v>13</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9">
+      <c r="N9">
         <v>11</v>
       </c>
+      <c r="O9" s="4"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="4"/>
@@ -995,10 +995,10 @@
       <c r="M10">
         <v>12</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10">
-        <v>10</v>
-      </c>
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="O10" s="4"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="1"/>
       <c r="R10">

</xml_diff>